<commit_message>
Finish Lesson 3 Hypothesis Testing and Problem Set in Udacity Inferential Stats
</commit_message>
<xml_diff>
--- a/Stats/Udacity/DataAnalystNanoDegree/IntroToInferentialStats/Lesson3_HypothesisTesting.xlsx
+++ b/Stats/Udacity/DataAnalystNanoDegree/IntroToInferentialStats/Lesson3_HypothesisTesting.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="7416" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="7416" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="quiz" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="49">
   <si>
     <t>SE</t>
   </si>
@@ -91,6 +92,100 @@
   </si>
   <si>
     <t>%</t>
+  </si>
+  <si>
+    <t>new p mean</t>
+  </si>
+  <si>
+    <t>&lt;--</t>
+  </si>
+  <si>
+    <t>= NOT STATISTICALLY SIG</t>
+  </si>
+  <si>
+    <t>is new pop parameter statistically sig?</t>
+  </si>
+  <si>
+    <t>new p z-score</t>
+  </si>
+  <si>
+    <t>sampl z-score</t>
+  </si>
+  <si>
+    <t>between 2 critical values of -1.96 and 1.96 = FAIL TO REJECT NULL</t>
+  </si>
+  <si>
+    <t>between 2 critical values of -1.96 and 1.96 = NULL IS TRUE</t>
+  </si>
+  <si>
+    <r>
+      <t>^^^</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>no errors</t>
+    </r>
+  </si>
+  <si>
+    <t>w/in critical value  1.96 = REJECT NULL</t>
+  </si>
+  <si>
+    <t>^^^TYPE I ERROR = randomly selected sample of already-more-engaged students</t>
+  </si>
+  <si>
+    <t>tails</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>z-crit</t>
+  </si>
+  <si>
+    <t>higher s mean = improve memory</t>
+  </si>
+  <si>
+    <t>mean z &gt; z-crit = reject null (that music won't affect memory and may make it worse)</t>
+  </si>
+  <si>
+    <t>Listening to music significantly improved memory at p &lt; 0.05</t>
+  </si>
+  <si>
+    <t>+/- 1.64</t>
+  </si>
+  <si>
+    <t>+/-1.64</t>
+  </si>
+  <si>
+    <t>mean z &lt; z-crit = reject null (that new training won't make runners faster and may make them slower)</t>
+  </si>
+  <si>
+    <t>lower  s mean = improve speed</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> new training significantly improved speed at p &lt; 0.05</t>
+  </si>
+  <si>
+    <t>+/- 2.32</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> new training significantly improved speed at p &lt; 0.01</t>
+  </si>
+  <si>
+    <t>p = 0.00001</t>
+  </si>
+  <si>
+    <t>p = 0.028002</t>
+  </si>
+  <si>
+    <t>p = 0.00135</t>
   </si>
 </sst>
 </file>
@@ -301,7 +396,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -338,6 +433,8 @@
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -747,16 +844,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I236"/>
+  <dimension ref="A1:K236"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="35.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1055,7 +1153,7 @@
         <v>0.72999999999999732</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="6">
         <v>41347.782905092594</v>
       </c>
@@ -1066,7 +1164,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="6">
         <v>41347.783090277779</v>
       </c>
@@ -1077,7 +1175,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="6">
         <v>41347.783877314818</v>
       </c>
@@ -1087,8 +1185,14 @@
       <c r="C19" s="8">
         <v>4</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E19" s="13">
+        <v>32</v>
+      </c>
+      <c r="F19" s="13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="6">
         <v>41347.784236111111</v>
       </c>
@@ -1098,8 +1202,14 @@
       <c r="C20" s="8">
         <v>5</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E20" t="s">
+        <v>5</v>
+      </c>
+      <c r="F20">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="6">
         <v>41347.785312499997</v>
       </c>
@@ -1109,8 +1219,14 @@
       <c r="C21" s="8">
         <v>8</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E21" t="s">
+        <v>12</v>
+      </c>
+      <c r="F21">
+        <v>8.3000000000000007</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="6">
         <v>41347.785381944443</v>
       </c>
@@ -1120,8 +1236,14 @@
       <c r="C22" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F22">
+        <v>7.8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="6">
         <v>41347.785879629628</v>
       </c>
@@ -1131,8 +1253,15 @@
       <c r="C23" s="8">
         <v>10</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E23" t="s">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <f>F3/SQRT(F20)</f>
+        <v>0.44054954227673582</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="6">
         <v>41347.786053240743</v>
       </c>
@@ -1142,8 +1271,24 @@
       <c r="C24" s="8">
         <v>6</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E24" t="s">
+        <v>27</v>
+      </c>
+      <c r="F24" s="13">
+        <f>(F21-F2)/F23</f>
+        <v>1.8835276272317956</v>
+      </c>
+      <c r="G24" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="H24" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="I24" s="13"/>
+      <c r="J24" s="13"/>
+      <c r="K24" s="13"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="6">
         <v>41347.787685185183</v>
       </c>
@@ -1153,8 +1298,15 @@
       <c r="C25" s="8">
         <v>4</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="G25" s="13"/>
+      <c r="H25" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="I25" s="13"/>
+      <c r="J25" s="13"/>
+      <c r="K25" s="13"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="6">
         <v>41347.788182870368</v>
       </c>
@@ -1164,8 +1316,24 @@
       <c r="C26" s="8">
         <v>8</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E26" t="s">
+        <v>26</v>
+      </c>
+      <c r="F26" s="13">
+        <f>(F22-F2)/F23</f>
+        <v>0.74858149287417408</v>
+      </c>
+      <c r="G26" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="H26" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="I26" s="13"/>
+      <c r="J26" s="13"/>
+      <c r="K26" s="13"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="6">
         <v>41347.788842592592</v>
       </c>
@@ -1175,8 +1343,13 @@
       <c r="C27" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="G27" s="13"/>
+      <c r="H27" s="14"/>
+      <c r="I27" s="13"/>
+      <c r="J27" s="13"/>
+      <c r="K27" s="13"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" s="6">
         <v>41347.790046296293</v>
       </c>
@@ -1186,8 +1359,11 @@
       <c r="C28" s="8">
         <v>7</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E28" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" s="6">
         <v>41347.790208333332</v>
       </c>
@@ -1198,7 +1374,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" s="6">
         <v>41347.791921296295</v>
       </c>
@@ -1208,8 +1384,14 @@
       <c r="C30" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E30" s="13">
+        <v>33</v>
+      </c>
+      <c r="F30" s="13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" s="6">
         <v>41347.793090277781</v>
       </c>
@@ -1219,8 +1401,14 @@
       <c r="C31" s="8">
         <v>2</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E31" t="s">
+        <v>5</v>
+      </c>
+      <c r="F31">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" s="6">
         <v>41347.79383101852</v>
       </c>
@@ -1230,8 +1418,14 @@
       <c r="C32" s="8">
         <v>6</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E32" t="s">
+        <v>12</v>
+      </c>
+      <c r="F32">
+        <v>8.3000000000000007</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" s="6">
         <v>41347.794409722221</v>
       </c>
@@ -1241,8 +1435,14 @@
       <c r="C33" s="8">
         <v>10</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E33" t="s">
+        <v>22</v>
+      </c>
+      <c r="F33">
+        <v>7.8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" s="6">
         <v>41347.798854166664</v>
       </c>
@@ -1252,8 +1452,15 @@
       <c r="C34" s="8">
         <v>9</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E34" t="s">
+        <v>0</v>
+      </c>
+      <c r="F34">
+        <f>F3/SQRT(F31)</f>
+        <v>0.34124820808341966</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" s="6">
         <v>41347.798888888887</v>
       </c>
@@ -1263,8 +1470,24 @@
       <c r="C35" s="8">
         <v>7</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E35" t="s">
+        <v>27</v>
+      </c>
+      <c r="F35" s="13">
+        <f>(F32-F2)/F34</f>
+        <v>2.4316237107967718</v>
+      </c>
+      <c r="G35" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="H35" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="I35" s="13"/>
+      <c r="J35" s="13"/>
+      <c r="K35" s="13"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" s="6">
         <v>41347.799004629633</v>
       </c>
@@ -1274,8 +1497,15 @@
       <c r="C36" s="8">
         <v>10</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="G36" s="13"/>
+      <c r="H36" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="I36" s="13"/>
+      <c r="J36" s="13"/>
+      <c r="K36" s="13"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" s="6">
         <v>41347.800266203703</v>
       </c>
@@ -1285,8 +1515,24 @@
       <c r="C37" s="8">
         <v>9</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E37" t="s">
+        <v>26</v>
+      </c>
+      <c r="F37" s="13">
+        <f>(F33-F2)/F34</f>
+        <v>0.96641455172692059</v>
+      </c>
+      <c r="G37" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="H37" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="I37" s="13"/>
+      <c r="J37" s="13"/>
+      <c r="K37" s="13"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38" s="6">
         <v>41347.800625000003</v>
       </c>
@@ -1297,7 +1543,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" s="6">
         <v>41347.804606481484</v>
       </c>
@@ -1307,8 +1553,11 @@
       <c r="C39" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E39" s="13" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40" s="6">
         <v>41347.806030092594</v>
       </c>
@@ -1319,7 +1568,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41" s="6">
         <v>41347.812361111108</v>
       </c>
@@ -1330,7 +1579,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42" s="6">
         <v>41347.813356481478</v>
       </c>
@@ -1341,7 +1590,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A43" s="6">
         <v>41347.814722222225</v>
       </c>
@@ -1352,7 +1601,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44" s="6">
         <v>41347.816736111112</v>
       </c>
@@ -1363,7 +1612,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45" s="6">
         <v>41347.819016203706</v>
       </c>
@@ -1374,7 +1623,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A46" s="6">
         <v>41347.81927083333</v>
       </c>
@@ -1385,7 +1634,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A47" s="6">
         <v>41347.819768518515</v>
       </c>
@@ -1396,7 +1645,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A48" s="6">
         <v>41347.821203703701</v>
       </c>
@@ -3473,6 +3722,283 @@
       </c>
       <c r="C236" s="11">
         <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>25</v>
+      </c>
+      <c r="D2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <f>B3/SQRT(B4)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="13">
+        <f>(B5-B2)/E2</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5">
+        <v>28</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6">
+        <v>0.05</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11">
+        <v>22.965</v>
+      </c>
+      <c r="D11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <f>B12/SQRT(B13)</f>
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12">
+        <v>0.36</v>
+      </c>
+      <c r="D12" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" s="13">
+        <f>(B14-B11)/E11</f>
+        <v>-1.9111111111111179</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <v>22.792999999999999</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>0.05</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>35</v>
+      </c>
+      <c r="B17" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>11</v>
+      </c>
+      <c r="B20">
+        <v>7895</v>
+      </c>
+      <c r="D20" t="s">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <f>B21/SQRT(B22)</f>
+        <v>102.85912696499032</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>1</v>
+      </c>
+      <c r="B21">
+        <v>230</v>
+      </c>
+      <c r="D21" t="s">
+        <v>13</v>
+      </c>
+      <c r="E21" s="13">
+        <f>(B23-B20)/E20</f>
+        <v>16.964950524944058</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>12</v>
+      </c>
+      <c r="B23">
+        <v>9640</v>
+      </c>
+      <c r="D23" s="13" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>14</v>
+      </c>
+      <c r="B24">
+        <v>0.01</v>
+      </c>
+      <c r="D24" s="13" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>33</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="D25" s="13" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>35</v>
+      </c>
+      <c r="B26" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="D26" s="13" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>